<commit_message>
Add better view for data
</commit_message>
<xml_diff>
--- a/scripts/PHPExcel/CSC Bonspiel.xlsx
+++ b/scripts/PHPExcel/CSC Bonspiel.xlsx
@@ -19,6 +19,7 @@
     <sheet name="DRAW MASTER INSTR." sheetId="12" state="hidden" r:id="rId10"/>
     <sheet name="1st draw times" sheetId="6" state="hidden" r:id="rId11"/>
     <sheet name="Data" sheetId="14" r:id="rId12"/>
+    <sheet name="Sheet1" sheetId="15" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Master Draw'!$O$2:$V$42</definedName>
@@ -112,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="357">
   <si>
     <t>FIRST EVENT</t>
   </si>
@@ -1161,12 +1162,6 @@
     <t>Saturday 8:00 AM</t>
   </si>
   <si>
-    <t>1st 1st</t>
-  </si>
-  <si>
-    <t>1st 2nd</t>
-  </si>
-  <si>
     <t>Saturday 3:00 PM</t>
   </si>
   <si>
@@ -1180,6 +1175,15 @@
   </si>
   <si>
     <t>ThisIsAVeryLongName</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>Bye</t>
   </si>
 </sst>
 </file>
@@ -2126,7 +2130,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="367">
+  <cellXfs count="368">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -2980,6 +2984,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3187,8 +3192,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A2:H32" totalsRowShown="0">
-  <autoFilter ref="A2:H32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A2:H34" totalsRowShown="0">
+  <autoFilter ref="A2:H34"/>
   <tableColumns count="8">
     <tableColumn id="1" name="1st Team"/>
     <tableColumn id="2" name="2nd Team"/>
@@ -5006,10 +5011,10 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5023,15 +5028,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="365" t="s">
+      <c r="A1" s="366" t="s">
         <v>347</v>
       </c>
-      <c r="B1" s="365"/>
-      <c r="C1" s="365"/>
-      <c r="D1" s="365"/>
-      <c r="E1" s="365"/>
-      <c r="F1" s="365"/>
-      <c r="G1" s="365"/>
+      <c r="B1" s="366"/>
+      <c r="C1" s="366"/>
+      <c r="D1" s="366"/>
+      <c r="E1" s="366"/>
+      <c r="F1" s="366"/>
+      <c r="G1" s="366"/>
+      <c r="H1" s="366"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
@@ -5061,7 +5067,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B3" t="s">
         <v>306</v>
@@ -5082,7 +5088,7 @@
         <v>201</v>
       </c>
       <c r="H3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -5450,434 +5456,456 @@
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" t="str">
+      <c r="A18" t="s">
+        <v>356</v>
+      </c>
+      <c r="E18">
+        <v>116</v>
+      </c>
+      <c r="H18" s="327"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="str">
         <f>H3</f>
         <v>ThisIsAVeryLongName</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B19" t="str">
         <f>H4</f>
         <v>T4</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>1</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D19" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>121</v>
       </c>
-      <c r="F18">
+      <c r="F19">
         <v>131</v>
       </c>
-      <c r="G18">
+      <c r="G19" s="327">
         <v>301</v>
       </c>
-      <c r="H18" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="str">
+      <c r="H19" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="str">
         <f>H5</f>
         <v>T6</v>
       </c>
-      <c r="B19" t="str">
+      <c r="B20" t="str">
         <f>H6</f>
         <v>T8</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>2</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D20" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>122</v>
       </c>
-      <c r="F19">
+      <c r="F20">
         <v>131</v>
       </c>
-      <c r="G19">
+      <c r="G20" s="327">
         <v>301</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="str">
+    <row r="21" spans="1:8">
+      <c r="A21" t="str">
         <f>H7</f>
         <v>T10</v>
       </c>
-      <c r="B20" t="str">
+      <c r="B21" t="str">
         <f>H8</f>
         <v>T12</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>3</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D21" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <v>123</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>132</v>
       </c>
-      <c r="G20">
+      <c r="G21" s="327">
         <v>302</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="str">
+    <row r="22" spans="1:8">
+      <c r="A22" t="str">
         <f>H9</f>
         <v>T14</v>
       </c>
-      <c r="B21" t="str">
+      <c r="B22" t="str">
         <f>H10</f>
         <v>T16</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>4</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D22" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>124</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>132</v>
       </c>
-      <c r="G21">
+      <c r="G22" s="327">
         <v>304</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H22" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="15" t="str">
+    <row r="23" spans="1:8">
+      <c r="A23" s="15" t="str">
         <f>H11</f>
         <v>T18</v>
       </c>
-      <c r="B22" s="15" t="str">
+      <c r="B23" s="15" t="str">
         <f>H12</f>
         <v>T20</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C23" s="15">
         <v>5</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D23" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E23" s="15">
         <v>125</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F23" s="15">
         <v>133</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G23" s="328">
         <v>303</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="H23" s="15" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" t="str">
+    <row r="24" spans="1:8">
+      <c r="A24" t="str">
         <f>H13</f>
         <v>T22</v>
       </c>
-      <c r="B23" t="str">
+      <c r="B24" t="str">
         <f>H14</f>
         <v>T24</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>1</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>343</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <v>126</v>
       </c>
-      <c r="F23">
+      <c r="F24">
         <v>133</v>
       </c>
-      <c r="G23">
+      <c r="G24" s="327">
         <v>303</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H24" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="325" t="str">
+    <row r="25" spans="1:8">
+      <c r="A25" s="325" t="str">
         <f>H15</f>
         <v>T26</v>
       </c>
-      <c r="B24" s="325" t="str">
+      <c r="B25" s="325" t="str">
         <f>H16</f>
         <v>T28</v>
       </c>
-      <c r="C24" s="325">
+      <c r="C25" s="325">
         <v>2</v>
       </c>
-      <c r="D24" s="325" t="s">
+      <c r="D25" s="325" t="s">
         <v>343</v>
       </c>
-      <c r="E24" s="325">
+      <c r="E25" s="325">
         <v>127</v>
       </c>
-      <c r="F24" s="325">
+      <c r="F25" s="325">
         <v>134</v>
       </c>
-      <c r="G24" s="325">
+      <c r="G25" s="329">
         <v>304</v>
       </c>
-      <c r="H24" s="325" t="s">
+      <c r="H25" s="325" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="str">
-        <f>H18</f>
-        <v>ThisIsAVeryLongName</v>
-      </c>
-      <c r="B25" t="str">
-        <f>H19</f>
-        <v>T8</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>348</v>
-      </c>
-      <c r="E25">
-        <v>131</v>
-      </c>
-      <c r="F25">
-        <v>141</v>
-      </c>
-      <c r="G25">
-        <v>501</v>
-      </c>
-      <c r="H25" s="327" t="s">
-        <v>355</v>
-      </c>
-    </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="15" t="str">
-        <f>H20</f>
-        <v>T12</v>
-      </c>
-      <c r="B26" s="15" t="str">
-        <f>H21</f>
-        <v>T16</v>
-      </c>
-      <c r="C26" s="15">
-        <v>2</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>348</v>
-      </c>
-      <c r="E26" s="15">
-        <v>132</v>
-      </c>
-      <c r="F26" s="15">
-        <v>141</v>
-      </c>
-      <c r="G26" s="15">
-        <v>511</v>
-      </c>
-      <c r="H26" s="328" t="s">
-        <v>320</v>
-      </c>
+      <c r="A26" t="s">
+        <v>356</v>
+      </c>
+      <c r="E26">
+        <v>128</v>
+      </c>
+      <c r="H26" s="327"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="str">
-        <f>H22</f>
-        <v>T20</v>
+        <f>H19</f>
+        <v>ThisIsAVeryLongName</v>
       </c>
       <c r="B27" t="str">
-        <f>H23</f>
-        <v>T24</v>
+        <f>H20</f>
+        <v>T8</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
         <v>348</v>
       </c>
       <c r="E27">
+        <v>131</v>
+      </c>
+      <c r="F27">
+        <v>141</v>
+      </c>
+      <c r="G27" s="327">
+        <v>501</v>
+      </c>
+      <c r="H27" s="327" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="15" t="str">
+        <f>H21</f>
+        <v>T12</v>
+      </c>
+      <c r="B28" s="15" t="str">
+        <f>H22</f>
+        <v>T16</v>
+      </c>
+      <c r="C28" s="15">
+        <v>2</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="E28" s="15">
+        <v>132</v>
+      </c>
+      <c r="F28" s="15">
+        <v>141</v>
+      </c>
+      <c r="G28" s="328">
+        <v>511</v>
+      </c>
+      <c r="H28" s="328" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="str">
+        <f>H23</f>
+        <v>T20</v>
+      </c>
+      <c r="B29" t="str">
+        <f>H24</f>
+        <v>T24</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>348</v>
+      </c>
+      <c r="E29">
         <v>133</v>
       </c>
-      <c r="F27">
+      <c r="F29">
         <v>142</v>
       </c>
-      <c r="G27">
+      <c r="G29" s="327">
         <v>501</v>
       </c>
-      <c r="H27" s="327" t="s">
+      <c r="H29" s="327" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="325" t="str">
-        <f>H24</f>
+    <row r="30" spans="1:8">
+      <c r="A30" s="325" t="str">
+        <f>H25</f>
         <v>T28</v>
       </c>
-      <c r="B28" s="325" t="str">
+      <c r="B30" s="325" t="str">
         <f>H17</f>
         <v>T30</v>
       </c>
-      <c r="C28" s="325">
+      <c r="C30" s="325">
         <v>4</v>
       </c>
-      <c r="D28" s="325" t="s">
+      <c r="D30" s="325" t="s">
         <v>348</v>
       </c>
-      <c r="E28" s="325">
+      <c r="E30" s="325">
         <v>134</v>
       </c>
-      <c r="F28" s="325">
+      <c r="F30" s="325">
         <v>142</v>
       </c>
-      <c r="G28" s="325">
+      <c r="G30" s="329">
         <v>302</v>
-      </c>
-      <c r="H28" s="325" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" t="str">
-        <f>H25</f>
-        <v>ThisIsAVeryLongName</v>
-      </c>
-      <c r="B29" t="str">
-        <f>H26</f>
-        <v>T16</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>351</v>
-      </c>
-      <c r="E29">
-        <v>141</v>
-      </c>
-      <c r="F29">
-        <v>161</v>
-      </c>
-      <c r="G29">
-        <v>151</v>
-      </c>
-      <c r="H29" s="327" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="325" t="str">
-        <f>H27</f>
-        <v>T24</v>
-      </c>
-      <c r="B30" s="325" t="str">
-        <f>H28</f>
-        <v>T30</v>
-      </c>
-      <c r="C30" s="325">
-        <v>2</v>
-      </c>
-      <c r="D30" s="325" t="s">
-        <v>351</v>
-      </c>
-      <c r="E30" s="325">
-        <v>142</v>
-      </c>
-      <c r="F30" s="325">
-        <v>161</v>
-      </c>
-      <c r="G30" s="325">
-        <v>151</v>
       </c>
       <c r="H30" s="325" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="325" t="str">
+      <c r="A31" t="str">
+        <f>H27</f>
+        <v>ThisIsAVeryLongName</v>
+      </c>
+      <c r="B31" t="str">
+        <f>H28</f>
+        <v>T16</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>349</v>
+      </c>
+      <c r="E31">
+        <v>141</v>
+      </c>
+      <c r="F31">
+        <v>161</v>
+      </c>
+      <c r="G31" s="327">
+        <v>151</v>
+      </c>
+      <c r="H31" s="327" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="325" t="str">
         <f>H29</f>
-        <v>ThisIsAVeryLongName</v>
-      </c>
-      <c r="B31" s="325" t="str">
+        <v>T24</v>
+      </c>
+      <c r="B32" s="325" t="str">
         <f>H30</f>
         <v>T30</v>
       </c>
-      <c r="C31" s="325">
+      <c r="C32" s="325">
+        <v>2</v>
+      </c>
+      <c r="D32" s="325" t="s">
+        <v>349</v>
+      </c>
+      <c r="E32" s="325">
+        <v>142</v>
+      </c>
+      <c r="F32" s="325">
+        <v>161</v>
+      </c>
+      <c r="G32" s="329">
+        <v>151</v>
+      </c>
+      <c r="H32" s="325" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="325" t="str">
+        <f>H31</f>
+        <v>T16</v>
+      </c>
+      <c r="B33" s="325" t="str">
+        <f>H32</f>
+        <v>T30</v>
+      </c>
+      <c r="C33" s="325">
         <v>3</v>
       </c>
-      <c r="D31" s="326" t="s">
+      <c r="D33" s="326" t="s">
+        <v>350</v>
+      </c>
+      <c r="E33" s="325">
+        <v>161</v>
+      </c>
+      <c r="F33" s="325" t="s">
+        <v>354</v>
+      </c>
+      <c r="G33" s="329" t="s">
+        <v>355</v>
+      </c>
+      <c r="H33" s="325" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="str">
+        <f>IF(H31="","",IF(H31=H27,H28,H27))</f>
+        <v>ThisIsAVeryLongName</v>
+      </c>
+      <c r="B34" t="str">
+        <f>IF(H32="","",IF(H32=H29,H30,H29))</f>
+        <v>T24</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="326" t="s">
+        <v>350</v>
+      </c>
+      <c r="E34">
+        <v>151</v>
+      </c>
+      <c r="F34" t="s">
+        <v>351</v>
+      </c>
+      <c r="G34" t="s">
         <v>352</v>
       </c>
-      <c r="E31" s="325">
-        <v>161</v>
-      </c>
-      <c r="F31" s="325" t="s">
-        <v>349</v>
-      </c>
-      <c r="G31" s="325" t="s">
-        <v>350</v>
-      </c>
-      <c r="H31" s="325" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" t="str">
-        <f>IF(H29="","",IF(H29=H25,H26,H25))</f>
-        <v>T16</v>
-      </c>
-      <c r="B32" t="str">
-        <f>IF(H30="","",IF(H30=H27,H28,H27))</f>
-        <v>T24</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" s="326" t="s">
-        <v>352</v>
-      </c>
-      <c r="E32">
-        <v>151</v>
-      </c>
-      <c r="F32" t="s">
-        <v>353</v>
-      </c>
-      <c r="G32" t="s">
-        <v>354</v>
-      </c>
-      <c r="H32" s="327" t="s">
+      <c r="H34" s="327" t="s">
         <v>328</v>
       </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="H35" s="327"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="F36" s="327"/>
+      <c r="H36" s="327"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="31">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H33:H1048576">
-      <formula1>"1"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3">
       <formula1>$A$3:$B$3</formula1>
     </dataValidation>
@@ -5923,9 +5951,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H17">
       <formula1>$A$17:$B$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H18">
-      <formula1>$A$18:$B$18</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H19">
       <formula1>$A$19:$B$19</formula1>
     </dataValidation>
@@ -5947,9 +5972,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H25">
       <formula1>$A$25:$B$25</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H26">
-      <formula1>$A$26:$B$26</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H27">
       <formula1>$A$27:$B$27</formula1>
     </dataValidation>
@@ -5968,12 +5990,33 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H32">
       <formula1>$A$32:$B$32</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H33">
+      <formula1>$A$33:$B$33</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H34">
+      <formula1>$A$34:$B$34</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H37:H1048576 F36">
+      <formula1>"1"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -8276,14 +8319,14 @@
       <c r="A20" s="242" t="s">
         <v>286</v>
       </c>
-      <c r="B20" s="329" t="s">
+      <c r="B20" s="330" t="s">
         <v>287</v>
       </c>
-      <c r="C20" s="330"/>
-      <c r="D20" s="330"/>
-      <c r="E20" s="330"/>
-      <c r="F20" s="330"/>
-      <c r="G20" s="330"/>
+      <c r="C20" s="331"/>
+      <c r="D20" s="331"/>
+      <c r="E20" s="331"/>
+      <c r="F20" s="331"/>
+      <c r="G20" s="331"/>
       <c r="H20" s="241"/>
     </row>
   </sheetData>
@@ -8303,8 +8346,8 @@
   </sheetPr>
   <dimension ref="A1:CB167"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" showZeros="0" topLeftCell="B1" zoomScale="63" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U33" sqref="U33"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" showZeros="0" topLeftCell="B11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -8392,13 +8435,13 @@
       <c r="U1" s="251"/>
       <c r="V1" s="251"/>
       <c r="W1" s="251"/>
-      <c r="AP1" s="361" t="s">
+      <c r="AP1" s="362" t="s">
         <v>184</v>
       </c>
-      <c r="AQ1" s="362"/>
-      <c r="AR1" s="362"/>
-      <c r="AS1" s="362"/>
-      <c r="AT1" s="363"/>
+      <c r="AQ1" s="363"/>
+      <c r="AR1" s="363"/>
+      <c r="AS1" s="363"/>
+      <c r="AT1" s="364"/>
       <c r="AV1" s="91">
         <v>0.33333333333333331</v>
       </c>
@@ -8537,7 +8580,7 @@
     </row>
     <row r="3" spans="1:65" ht="18" customHeight="1">
       <c r="A3" s="245"/>
-      <c r="B3" s="352">
+      <c r="B3" s="353">
         <v>101</v>
       </c>
       <c r="C3" s="255" t="s">
@@ -8563,7 +8606,7 @@
       <c r="U3" s="256" t="s">
         <v>191</v>
       </c>
-      <c r="V3" s="354">
+      <c r="V3" s="355">
         <v>109</v>
       </c>
       <c r="W3" s="257"/>
@@ -8643,7 +8686,7 @@
     </row>
     <row r="4" spans="1:65" ht="18" customHeight="1" thickBot="1">
       <c r="A4" s="245"/>
-      <c r="B4" s="344"/>
+      <c r="B4" s="345"/>
       <c r="C4" s="258" t="s">
         <v>256</v>
       </c>
@@ -8667,7 +8710,7 @@
       <c r="U4" s="261" t="s">
         <v>197</v>
       </c>
-      <c r="V4" s="345"/>
+      <c r="V4" s="346"/>
       <c r="W4" s="257"/>
       <c r="X4" s="318" t="str">
         <f>B6</f>
@@ -8745,7 +8788,7 @@
     </row>
     <row r="5" spans="1:65" ht="18" customHeight="1" thickBot="1">
       <c r="A5" s="245"/>
-      <c r="B5" s="353"/>
+      <c r="B5" s="354"/>
       <c r="C5" s="262" t="s">
         <v>5</v>
       </c>
@@ -8769,7 +8812,7 @@
       <c r="U5" s="268" t="s">
         <v>63</v>
       </c>
-      <c r="V5" s="355"/>
+      <c r="V5" s="356"/>
       <c r="W5" s="257"/>
       <c r="X5" s="318" t="str">
         <f>B8</f>
@@ -8852,7 +8895,7 @@
         <v>T2</v>
       </c>
       <c r="C6" s="315"/>
-      <c r="D6" s="344">
+      <c r="D6" s="345">
         <v>121</v>
       </c>
       <c r="E6" s="269" t="s">
@@ -8874,7 +8917,7 @@
       <c r="S6" s="316" t="s">
         <v>215</v>
       </c>
-      <c r="T6" s="345">
+      <c r="T6" s="346">
         <v>125</v>
       </c>
       <c r="U6" s="250"/>
@@ -8906,13 +8949,13 @@
       <c r="AL6" s="198"/>
       <c r="AM6" s="198"/>
       <c r="AO6" s="136"/>
-      <c r="AP6" s="356" t="s">
+      <c r="AP6" s="357" t="s">
         <v>206</v>
       </c>
-      <c r="AQ6" s="357"/>
-      <c r="AR6" s="357"/>
-      <c r="AS6" s="357"/>
-      <c r="AT6" s="358"/>
+      <c r="AQ6" s="358"/>
+      <c r="AR6" s="358"/>
+      <c r="AS6" s="358"/>
+      <c r="AT6" s="359"/>
       <c r="AV6" s="91">
         <v>0.42708333333333331</v>
       </c>
@@ -8957,7 +9000,7 @@
       <c r="A7" s="245"/>
       <c r="B7" s="246"/>
       <c r="C7" s="247"/>
-      <c r="D7" s="344"/>
+      <c r="D7" s="345"/>
       <c r="E7" s="269" t="s">
         <v>207</v>
       </c>
@@ -8977,7 +9020,7 @@
       <c r="S7" s="316" t="s">
         <v>207</v>
       </c>
-      <c r="T7" s="345"/>
+      <c r="T7" s="346"/>
       <c r="U7" s="251"/>
       <c r="V7" s="251"/>
       <c r="W7" s="251"/>
@@ -9051,7 +9094,7 @@
         <v>T3</v>
       </c>
       <c r="C8" s="252"/>
-      <c r="D8" s="344"/>
+      <c r="D8" s="345"/>
       <c r="E8" s="269" t="s">
         <v>14</v>
       </c>
@@ -9071,7 +9114,7 @@
       <c r="S8" s="316" t="s">
         <v>67</v>
       </c>
-      <c r="T8" s="345"/>
+      <c r="T8" s="346"/>
       <c r="U8" s="250"/>
       <c r="V8" s="251" t="str">
         <f>Data!A12</f>
@@ -9130,7 +9173,7 @@
     </row>
     <row r="9" spans="1:65" ht="18" customHeight="1" thickBot="1">
       <c r="A9" s="245"/>
-      <c r="B9" s="352">
+      <c r="B9" s="353">
         <v>102</v>
       </c>
       <c r="C9" s="255" t="s">
@@ -9156,7 +9199,7 @@
       <c r="U9" s="256" t="s">
         <v>216</v>
       </c>
-      <c r="V9" s="354">
+      <c r="V9" s="355">
         <v>110</v>
       </c>
       <c r="W9" s="257"/>
@@ -9226,7 +9269,7 @@
     </row>
     <row r="10" spans="1:65" ht="18" customHeight="1">
       <c r="A10" s="245"/>
-      <c r="B10" s="344"/>
+      <c r="B10" s="345"/>
       <c r="C10" s="258" t="s">
         <v>197</v>
       </c>
@@ -9250,7 +9293,7 @@
       <c r="U10" s="261" t="s">
         <v>197</v>
       </c>
-      <c r="V10" s="345"/>
+      <c r="V10" s="346"/>
       <c r="W10" s="257"/>
       <c r="X10" s="318" t="str">
         <f>B24</f>
@@ -9316,7 +9359,7 @@
     </row>
     <row r="11" spans="1:65" ht="18" customHeight="1" thickBot="1">
       <c r="A11" s="245"/>
-      <c r="B11" s="353"/>
+      <c r="B11" s="354"/>
       <c r="C11" s="262" t="s">
         <v>5</v>
       </c>
@@ -9340,7 +9383,7 @@
       <c r="U11" s="268" t="s">
         <v>63</v>
       </c>
-      <c r="V11" s="355"/>
+      <c r="V11" s="356"/>
       <c r="W11" s="257"/>
       <c r="X11" s="318" t="str">
         <f>B26</f>
@@ -9421,7 +9464,7 @@
       <c r="C12" s="315"/>
       <c r="D12" s="249"/>
       <c r="E12" s="249"/>
-      <c r="F12" s="344">
+      <c r="F12" s="345">
         <v>131</v>
       </c>
       <c r="G12" s="269" t="s">
@@ -9439,7 +9482,7 @@
       <c r="Q12" s="316" t="s">
         <v>215</v>
       </c>
-      <c r="R12" s="345">
+      <c r="R12" s="346">
         <v>133</v>
       </c>
       <c r="S12" s="251"/>
@@ -9503,7 +9546,7 @@
       <c r="C13" s="247"/>
       <c r="D13" s="248"/>
       <c r="E13" s="248"/>
-      <c r="F13" s="344"/>
+      <c r="F13" s="345"/>
       <c r="G13" s="269" t="s">
         <v>247</v>
       </c>
@@ -9521,7 +9564,7 @@
       <c r="Q13" s="276" t="s">
         <v>247</v>
       </c>
-      <c r="R13" s="345"/>
+      <c r="R13" s="346"/>
       <c r="S13" s="251"/>
       <c r="T13" s="251"/>
       <c r="U13" s="251"/>
@@ -9536,13 +9579,13 @@
         <v>0</v>
       </c>
       <c r="AO13" s="136"/>
-      <c r="AP13" s="356" t="s">
+      <c r="AP13" s="357" t="s">
         <v>206</v>
       </c>
-      <c r="AQ13" s="357"/>
-      <c r="AR13" s="357"/>
-      <c r="AS13" s="357"/>
-      <c r="AT13" s="358"/>
+      <c r="AQ13" s="358"/>
+      <c r="AR13" s="358"/>
+      <c r="AS13" s="358"/>
+      <c r="AT13" s="359"/>
       <c r="AW13" s="92">
         <v>113</v>
       </c>
@@ -9573,7 +9616,7 @@
       <c r="C14" s="252"/>
       <c r="D14" s="248"/>
       <c r="E14" s="248"/>
-      <c r="F14" s="344"/>
+      <c r="F14" s="345"/>
       <c r="G14" s="269" t="s">
         <v>21</v>
       </c>
@@ -9589,7 +9632,7 @@
       <c r="Q14" s="316" t="s">
         <v>21</v>
       </c>
-      <c r="R14" s="345"/>
+      <c r="R14" s="346"/>
       <c r="S14" s="251"/>
       <c r="T14" s="251"/>
       <c r="U14" s="250"/>
@@ -9645,7 +9688,7 @@
     </row>
     <row r="15" spans="1:65" ht="18" customHeight="1" thickBot="1">
       <c r="A15" s="282"/>
-      <c r="B15" s="352">
+      <c r="B15" s="353">
         <v>103</v>
       </c>
       <c r="C15" s="255" t="s">
@@ -9671,7 +9714,7 @@
       <c r="U15" s="256" t="s">
         <v>205</v>
       </c>
-      <c r="V15" s="354">
+      <c r="V15" s="355">
         <v>111</v>
       </c>
       <c r="W15" s="257"/>
@@ -9736,7 +9779,7 @@
     </row>
     <row r="16" spans="1:65" ht="18" customHeight="1" thickBot="1">
       <c r="A16" s="282"/>
-      <c r="B16" s="344"/>
+      <c r="B16" s="345"/>
       <c r="C16" s="258" t="s">
         <v>197</v>
       </c>
@@ -9760,7 +9803,7 @@
       <c r="U16" s="261" t="s">
         <v>198</v>
       </c>
-      <c r="V16" s="345"/>
+      <c r="V16" s="346"/>
       <c r="W16" s="257"/>
       <c r="X16" s="318" t="str">
         <f>B42</f>
@@ -9818,7 +9861,7 @@
     </row>
     <row r="17" spans="1:65" ht="18" customHeight="1" thickBot="1">
       <c r="A17" s="282"/>
-      <c r="B17" s="353"/>
+      <c r="B17" s="354"/>
       <c r="C17" s="262" t="s">
         <v>22</v>
       </c>
@@ -9842,7 +9885,7 @@
       <c r="U17" s="268" t="s">
         <v>73</v>
       </c>
-      <c r="V17" s="355"/>
+      <c r="V17" s="356"/>
       <c r="W17" s="257"/>
       <c r="X17" s="318" t="str">
         <f>B44</f>
@@ -9867,13 +9910,13 @@
       <c r="AL17" s="200"/>
       <c r="AM17" s="200"/>
       <c r="AO17" s="136"/>
-      <c r="AP17" s="356" t="s">
+      <c r="AP17" s="357" t="s">
         <v>206</v>
       </c>
-      <c r="AQ17" s="357"/>
-      <c r="AR17" s="357"/>
-      <c r="AS17" s="357"/>
-      <c r="AT17" s="358"/>
+      <c r="AQ17" s="358"/>
+      <c r="AR17" s="358"/>
+      <c r="AS17" s="358"/>
+      <c r="AT17" s="359"/>
       <c r="AV17" s="91">
         <v>0.625</v>
       </c>
@@ -9904,7 +9947,7 @@
         <v>T6</v>
       </c>
       <c r="C18" s="315"/>
-      <c r="D18" s="344">
+      <c r="D18" s="345">
         <v>122</v>
       </c>
       <c r="E18" s="269" t="s">
@@ -9926,7 +9969,7 @@
       <c r="S18" s="316" t="s">
         <v>190</v>
       </c>
-      <c r="T18" s="345">
+      <c r="T18" s="346">
         <v>126</v>
       </c>
       <c r="U18" s="250"/>
@@ -9980,7 +10023,7 @@
       <c r="A19" s="282"/>
       <c r="B19" s="313"/>
       <c r="C19" s="247"/>
-      <c r="D19" s="344"/>
+      <c r="D19" s="345"/>
       <c r="E19" s="269" t="s">
         <v>207</v>
       </c>
@@ -10000,7 +10043,7 @@
       <c r="S19" s="316" t="s">
         <v>208</v>
       </c>
-      <c r="T19" s="345"/>
+      <c r="T19" s="346"/>
       <c r="U19" s="251"/>
       <c r="V19" s="251"/>
       <c r="W19" s="251"/>
@@ -10036,7 +10079,7 @@
         <v>T7</v>
       </c>
       <c r="C20" s="252"/>
-      <c r="D20" s="344"/>
+      <c r="D20" s="345"/>
       <c r="E20" s="269" t="s">
         <v>14</v>
       </c>
@@ -10056,7 +10099,7 @@
       <c r="S20" s="316" t="s">
         <v>67</v>
       </c>
-      <c r="T20" s="345"/>
+      <c r="T20" s="346"/>
       <c r="U20" s="250"/>
       <c r="V20" s="251" t="str">
         <f>Data!A14</f>
@@ -10090,7 +10133,7 @@
     </row>
     <row r="21" spans="1:65" ht="18" customHeight="1" thickBot="1">
       <c r="A21" s="282"/>
-      <c r="B21" s="352">
+      <c r="B21" s="353">
         <v>104</v>
       </c>
       <c r="C21" s="255" t="s">
@@ -10118,7 +10161,7 @@
       <c r="U21" s="256" t="s">
         <v>191</v>
       </c>
-      <c r="V21" s="354">
+      <c r="V21" s="355">
         <v>112</v>
       </c>
       <c r="W21" s="257"/>
@@ -10163,7 +10206,7 @@
     </row>
     <row r="22" spans="1:65" ht="18" customHeight="1">
       <c r="A22" s="292"/>
-      <c r="B22" s="344"/>
+      <c r="B22" s="345"/>
       <c r="C22" s="258" t="s">
         <v>198</v>
       </c>
@@ -10189,7 +10232,7 @@
       <c r="U22" s="261" t="s">
         <v>198</v>
       </c>
-      <c r="V22" s="345"/>
+      <c r="V22" s="346"/>
       <c r="W22" s="257"/>
       <c r="X22" s="318" t="str">
         <f>V12</f>
@@ -10238,7 +10281,7 @@
     </row>
     <row r="23" spans="1:65" ht="18" customHeight="1" thickBot="1">
       <c r="A23" s="293"/>
-      <c r="B23" s="353"/>
+      <c r="B23" s="354"/>
       <c r="C23" s="262" t="s">
         <v>22</v>
       </c>
@@ -10264,7 +10307,7 @@
       <c r="U23" s="268" t="s">
         <v>73</v>
       </c>
-      <c r="V23" s="355"/>
+      <c r="V23" s="356"/>
       <c r="W23" s="257"/>
       <c r="X23" s="318" t="str">
         <f>V14</f>
@@ -10316,7 +10359,7 @@
       <c r="E24" s="248"/>
       <c r="F24" s="249"/>
       <c r="G24" s="249"/>
-      <c r="H24" s="344">
+      <c r="H24" s="345">
         <v>141</v>
       </c>
       <c r="I24" s="288" t="s">
@@ -10330,7 +10373,7 @@
       <c r="O24" s="316" t="s">
         <v>216</v>
       </c>
-      <c r="P24" s="345">
+      <c r="P24" s="346">
         <v>142</v>
       </c>
       <c r="Q24" s="251"/>
@@ -10374,7 +10417,7 @@
       <c r="E25" s="248"/>
       <c r="F25" s="249"/>
       <c r="G25" s="249"/>
-      <c r="H25" s="344"/>
+      <c r="H25" s="345"/>
       <c r="I25" s="288" t="s">
         <v>250</v>
       </c>
@@ -10386,7 +10429,7 @@
       <c r="O25" s="316" t="s">
         <v>250</v>
       </c>
-      <c r="P25" s="345"/>
+      <c r="P25" s="346"/>
       <c r="Q25" s="251"/>
       <c r="R25" s="251"/>
       <c r="S25" s="251"/>
@@ -10430,7 +10473,7 @@
       <c r="E26" s="248"/>
       <c r="F26" s="249"/>
       <c r="G26" s="249"/>
-      <c r="H26" s="344"/>
+      <c r="H26" s="345"/>
       <c r="I26" s="258" t="s">
         <v>33</v>
       </c>
@@ -10442,7 +10485,7 @@
       <c r="O26" s="316" t="s">
         <v>33</v>
       </c>
-      <c r="P26" s="345"/>
+      <c r="P26" s="346"/>
       <c r="Q26" s="251"/>
       <c r="R26" s="251"/>
       <c r="S26" s="251"/>
@@ -10480,7 +10523,7 @@
     </row>
     <row r="27" spans="1:65" ht="18" customHeight="1">
       <c r="A27" s="294"/>
-      <c r="B27" s="352">
+      <c r="B27" s="353">
         <v>105</v>
       </c>
       <c r="C27" s="255" t="s">
@@ -10506,7 +10549,7 @@
       <c r="U27" s="256" t="s">
         <v>216</v>
       </c>
-      <c r="V27" s="354">
+      <c r="V27" s="355">
         <v>113</v>
       </c>
       <c r="W27" s="257"/>
@@ -10552,7 +10595,7 @@
     </row>
     <row r="28" spans="1:65" ht="18" customHeight="1" thickBot="1">
       <c r="A28" s="294"/>
-      <c r="B28" s="344"/>
+      <c r="B28" s="345"/>
       <c r="C28" s="258" t="s">
         <v>198</v>
       </c>
@@ -10576,7 +10619,7 @@
       <c r="U28" s="261" t="s">
         <v>198</v>
       </c>
-      <c r="V28" s="345"/>
+      <c r="V28" s="346"/>
       <c r="W28" s="257"/>
       <c r="X28" s="318" t="str">
         <f>V30</f>
@@ -10616,7 +10659,7 @@
     </row>
     <row r="29" spans="1:65" ht="18" customHeight="1" thickBot="1">
       <c r="A29" s="294"/>
-      <c r="B29" s="353"/>
+      <c r="B29" s="354"/>
       <c r="C29" s="262" t="s">
         <v>35</v>
       </c>
@@ -10627,11 +10670,11 @@
       <c r="H29" s="287"/>
       <c r="I29" s="288"/>
       <c r="J29" s="250"/>
-      <c r="K29" s="359" t="s">
+      <c r="K29" s="360" t="s">
         <v>242</v>
       </c>
-      <c r="L29" s="360"/>
-      <c r="M29" s="360"/>
+      <c r="L29" s="361"/>
+      <c r="M29" s="361"/>
       <c r="N29" s="250"/>
       <c r="O29" s="316"/>
       <c r="P29" s="276"/>
@@ -10642,7 +10685,7 @@
       <c r="U29" s="268" t="s">
         <v>82</v>
       </c>
-      <c r="V29" s="355"/>
+      <c r="V29" s="356"/>
       <c r="W29" s="257"/>
       <c r="X29" s="318" t="str">
         <f>V32</f>
@@ -10686,7 +10729,7 @@
         <v>T10</v>
       </c>
       <c r="C30" s="315"/>
-      <c r="D30" s="344">
+      <c r="D30" s="345">
         <v>123</v>
       </c>
       <c r="E30" s="269" t="s">
@@ -10708,7 +10751,7 @@
       <c r="S30" s="316" t="s">
         <v>205</v>
       </c>
-      <c r="T30" s="345">
+      <c r="T30" s="346">
         <v>127</v>
       </c>
       <c r="U30" s="250"/>
@@ -10746,7 +10789,7 @@
       <c r="A31" s="300"/>
       <c r="B31" s="246"/>
       <c r="C31" s="247"/>
-      <c r="D31" s="344"/>
+      <c r="D31" s="345"/>
       <c r="E31" s="269" t="s">
         <v>208</v>
       </c>
@@ -10766,7 +10809,7 @@
       <c r="S31" s="316" t="s">
         <v>234</v>
       </c>
-      <c r="T31" s="345"/>
+      <c r="T31" s="346"/>
       <c r="U31" s="251"/>
       <c r="V31" s="251"/>
       <c r="W31" s="251"/>
@@ -10795,7 +10838,7 @@
         <v>T11</v>
       </c>
       <c r="C32" s="252"/>
-      <c r="D32" s="344"/>
+      <c r="D32" s="345"/>
       <c r="E32" s="269" t="s">
         <v>40</v>
       </c>
@@ -10815,7 +10858,7 @@
       <c r="S32" s="316" t="s">
         <v>55</v>
       </c>
-      <c r="T32" s="345"/>
+      <c r="T32" s="346"/>
       <c r="U32" s="250"/>
       <c r="V32" s="251" t="str">
         <f>Data!A16</f>
@@ -10839,7 +10882,7 @@
     </row>
     <row r="33" spans="1:61" ht="18" customHeight="1" thickBot="1">
       <c r="A33" s="299"/>
-      <c r="B33" s="352">
+      <c r="B33" s="353">
         <v>106</v>
       </c>
       <c r="C33" s="255" t="s">
@@ -10865,7 +10908,7 @@
       <c r="U33" s="256" t="s">
         <v>216</v>
       </c>
-      <c r="V33" s="354">
+      <c r="V33" s="355">
         <v>114</v>
       </c>
       <c r="W33" s="257"/>
@@ -10888,7 +10931,7 @@
     </row>
     <row r="34" spans="1:61" ht="18" customHeight="1">
       <c r="A34" s="245"/>
-      <c r="B34" s="344"/>
+      <c r="B34" s="345"/>
       <c r="C34" s="306" t="s">
         <v>230</v>
       </c>
@@ -10912,7 +10955,7 @@
       <c r="U34" s="261" t="s">
         <v>230</v>
       </c>
-      <c r="V34" s="345"/>
+      <c r="V34" s="346"/>
       <c r="W34" s="257"/>
       <c r="X34" s="200"/>
       <c r="Y34" s="200"/>
@@ -10945,7 +10988,7 @@
     </row>
     <row r="35" spans="1:61" ht="18" customHeight="1" thickBot="1">
       <c r="A35" s="245"/>
-      <c r="B35" s="353"/>
+      <c r="B35" s="354"/>
       <c r="C35" s="262" t="s">
         <v>35</v>
       </c>
@@ -10969,7 +11012,7 @@
       <c r="U35" s="268" t="s">
         <v>82</v>
       </c>
-      <c r="V35" s="355"/>
+      <c r="V35" s="356"/>
       <c r="W35" s="257"/>
       <c r="X35" s="200"/>
       <c r="Y35" s="200"/>
@@ -10997,7 +11040,7 @@
       <c r="C36" s="315"/>
       <c r="D36" s="249"/>
       <c r="E36" s="249"/>
-      <c r="F36" s="344">
+      <c r="F36" s="345">
         <v>132</v>
       </c>
       <c r="G36" s="269" t="s">
@@ -11015,7 +11058,7 @@
       <c r="Q36" s="316" t="s">
         <v>190</v>
       </c>
-      <c r="R36" s="345">
+      <c r="R36" s="346">
         <v>134</v>
       </c>
       <c r="S36" s="251"/>
@@ -11034,7 +11077,7 @@
       <c r="C37" s="247"/>
       <c r="D37" s="248"/>
       <c r="E37" s="248"/>
-      <c r="F37" s="344"/>
+      <c r="F37" s="345"/>
       <c r="G37" s="269" t="s">
         <v>223</v>
       </c>
@@ -11050,7 +11093,7 @@
       <c r="Q37" s="316" t="s">
         <v>223</v>
       </c>
-      <c r="R37" s="345"/>
+      <c r="R37" s="346"/>
       <c r="S37" s="251"/>
       <c r="T37" s="251"/>
       <c r="U37" s="251"/>
@@ -11067,7 +11110,7 @@
       <c r="C38" s="252"/>
       <c r="D38" s="248"/>
       <c r="E38" s="248"/>
-      <c r="F38" s="344"/>
+      <c r="F38" s="345"/>
       <c r="G38" s="269" t="s">
         <v>48</v>
       </c>
@@ -11085,7 +11128,7 @@
       <c r="Q38" s="316" t="s">
         <v>40</v>
       </c>
-      <c r="R38" s="345"/>
+      <c r="R38" s="346"/>
       <c r="S38" s="251"/>
       <c r="T38" s="251"/>
       <c r="U38" s="250"/>
@@ -11099,7 +11142,7 @@
     </row>
     <row r="39" spans="1:61" ht="18" customHeight="1">
       <c r="A39" s="245"/>
-      <c r="B39" s="352">
+      <c r="B39" s="353">
         <v>107</v>
       </c>
       <c r="C39" s="255" t="s">
@@ -11127,7 +11170,7 @@
       <c r="U39" s="256" t="s">
         <v>191</v>
       </c>
-      <c r="V39" s="354">
+      <c r="V39" s="355">
         <v>115</v>
       </c>
       <c r="W39" s="257"/>
@@ -11152,7 +11195,7 @@
     </row>
     <row r="40" spans="1:61" ht="18" customHeight="1" thickBot="1">
       <c r="A40" s="245"/>
-      <c r="B40" s="344"/>
+      <c r="B40" s="345"/>
       <c r="C40" s="306" t="s">
         <v>230</v>
       </c>
@@ -11178,7 +11221,7 @@
       <c r="U40" s="261" t="s">
         <v>230</v>
       </c>
-      <c r="V40" s="345"/>
+      <c r="V40" s="346"/>
       <c r="W40" s="257"/>
       <c r="X40" s="200"/>
       <c r="Y40" s="200"/>
@@ -11201,7 +11244,7 @@
     </row>
     <row r="41" spans="1:61" ht="18" customHeight="1" thickBot="1">
       <c r="A41" s="245"/>
-      <c r="B41" s="353"/>
+      <c r="B41" s="354"/>
       <c r="C41" s="262" t="s">
         <v>50</v>
       </c>
@@ -11225,7 +11268,7 @@
       <c r="U41" s="268" t="s">
         <v>91</v>
       </c>
-      <c r="V41" s="355"/>
+      <c r="V41" s="356"/>
       <c r="W41" s="257"/>
       <c r="X41" s="200"/>
       <c r="Y41" s="200"/>
@@ -11253,7 +11296,7 @@
         <v>T14</v>
       </c>
       <c r="C42" s="315"/>
-      <c r="D42" s="344">
+      <c r="D42" s="345">
         <v>124</v>
       </c>
       <c r="E42" s="269" t="s">
@@ -11275,7 +11318,7 @@
       <c r="Q42" s="276"/>
       <c r="R42" s="276"/>
       <c r="S42" s="276"/>
-      <c r="T42" s="345"/>
+      <c r="T42" s="346"/>
       <c r="U42" s="250"/>
       <c r="V42" s="86" t="str">
         <f>Data!B17</f>
@@ -11289,7 +11332,7 @@
       <c r="A43" s="245"/>
       <c r="B43" s="246"/>
       <c r="C43" s="247"/>
-      <c r="D43" s="344"/>
+      <c r="D43" s="345"/>
       <c r="E43" s="306" t="s">
         <v>234</v>
       </c>
@@ -11307,7 +11350,7 @@
       <c r="Q43" s="276"/>
       <c r="R43" s="276"/>
       <c r="S43" s="276"/>
-      <c r="T43" s="345"/>
+      <c r="T43" s="346"/>
       <c r="U43" s="251"/>
       <c r="V43" s="251"/>
       <c r="W43" s="251"/>
@@ -11320,7 +11363,7 @@
         <v>T15</v>
       </c>
       <c r="C44" s="252"/>
-      <c r="D44" s="344"/>
+      <c r="D44" s="345"/>
       <c r="E44" s="269" t="s">
         <v>55</v>
       </c>
@@ -11338,7 +11381,7 @@
       <c r="Q44" s="251"/>
       <c r="R44" s="251"/>
       <c r="S44" s="276"/>
-      <c r="T44" s="345"/>
+      <c r="T44" s="346"/>
       <c r="U44" s="287"/>
       <c r="V44" s="276"/>
       <c r="W44" s="276"/>
@@ -11362,7 +11405,7 @@
     </row>
     <row r="45" spans="1:61" ht="18" customHeight="1" thickBot="1">
       <c r="A45" s="299"/>
-      <c r="B45" s="352">
+      <c r="B45" s="353">
         <v>108</v>
       </c>
       <c r="C45" s="255" t="s">
@@ -11379,11 +11422,11 @@
         <v/>
       </c>
       <c r="K45" s="312"/>
-      <c r="L45" s="350" t="s">
+      <c r="L45" s="351" t="s">
         <v>244</v>
       </c>
-      <c r="M45" s="351"/>
-      <c r="N45" s="351"/>
+      <c r="M45" s="352"/>
+      <c r="N45" s="352"/>
       <c r="O45" s="251"/>
       <c r="P45" s="251"/>
       <c r="Q45" s="251"/>
@@ -11391,7 +11434,7 @@
       <c r="S45" s="276"/>
       <c r="T45" s="276"/>
       <c r="U45" s="254"/>
-      <c r="V45" s="345"/>
+      <c r="V45" s="346"/>
       <c r="W45" s="257"/>
       <c r="X45" s="200"/>
       <c r="Y45" s="200"/>
@@ -11413,7 +11456,7 @@
     </row>
     <row r="46" spans="1:61" ht="18" customHeight="1">
       <c r="A46" s="294"/>
-      <c r="B46" s="344"/>
+      <c r="B46" s="345"/>
       <c r="C46" s="306" t="s">
         <v>230</v>
       </c>
@@ -11423,12 +11466,12 @@
       <c r="G46" s="249"/>
       <c r="H46" s="250"/>
       <c r="I46" s="250"/>
-      <c r="J46" s="346"/>
-      <c r="K46" s="347"/>
-      <c r="L46" s="348" t="s">
+      <c r="J46" s="347"/>
+      <c r="K46" s="348"/>
+      <c r="L46" s="349" t="s">
         <v>304</v>
       </c>
-      <c r="M46" s="349"/>
+      <c r="M46" s="350"/>
       <c r="N46" s="250"/>
       <c r="O46" s="251"/>
       <c r="P46" s="251"/>
@@ -11437,7 +11480,7 @@
       <c r="S46" s="251"/>
       <c r="T46" s="251"/>
       <c r="U46" s="254"/>
-      <c r="V46" s="345"/>
+      <c r="V46" s="346"/>
       <c r="W46" s="257"/>
       <c r="X46" s="200"/>
       <c r="Y46" s="200"/>
@@ -11460,7 +11503,7 @@
     </row>
     <row r="47" spans="1:61" ht="18" customHeight="1" thickBot="1">
       <c r="A47" s="294"/>
-      <c r="B47" s="353"/>
+      <c r="B47" s="354"/>
       <c r="C47" s="262" t="s">
         <v>50</v>
       </c>
@@ -11482,7 +11525,7 @@
       <c r="S47" s="251"/>
       <c r="T47" s="251"/>
       <c r="U47" s="254"/>
-      <c r="V47" s="345"/>
+      <c r="V47" s="346"/>
       <c r="W47" s="257"/>
       <c r="X47" s="200"/>
       <c r="Y47" s="200"/>
@@ -11976,7 +12019,7 @@
     <row r="74" spans="1:80" ht="13.5" customHeight="1">
       <c r="B74" s="80"/>
       <c r="C74" s="80"/>
-      <c r="D74" s="338">
+      <c r="D74" s="339">
         <v>201</v>
       </c>
       <c r="E74" s="106" t="s">
@@ -11989,14 +12032,14 @@
       <c r="S74" s="107" t="s">
         <v>190</v>
       </c>
-      <c r="T74" s="340">
+      <c r="T74" s="341">
         <v>205</v>
       </c>
     </row>
     <row r="75" spans="1:80" ht="13.5" customHeight="1" thickBot="1">
       <c r="B75" s="80"/>
       <c r="C75" s="80"/>
-      <c r="D75" s="333"/>
+      <c r="D75" s="334"/>
       <c r="E75" s="112" t="s">
         <v>207</v>
       </c>
@@ -12012,12 +12055,12 @@
       <c r="S75" s="113" t="s">
         <v>207</v>
       </c>
-      <c r="T75" s="334"/>
+      <c r="T75" s="335"/>
     </row>
     <row r="76" spans="1:80" ht="13.5" customHeight="1" thickBot="1">
       <c r="B76" s="80"/>
       <c r="C76" s="80"/>
-      <c r="D76" s="339"/>
+      <c r="D76" s="340"/>
       <c r="E76" s="120" t="s">
         <v>95</v>
       </c>
@@ -12030,7 +12073,7 @@
       <c r="S76" s="126" t="s">
         <v>105</v>
       </c>
-      <c r="T76" s="341"/>
+      <c r="T76" s="342"/>
     </row>
     <row r="77" spans="1:80" ht="13.5" customHeight="1">
       <c r="B77" s="80"/>
@@ -12040,7 +12083,7 @@
         <v/>
       </c>
       <c r="E77" s="133"/>
-      <c r="F77" s="333">
+      <c r="F77" s="334">
         <v>211</v>
       </c>
       <c r="G77" s="134" t="s">
@@ -12051,7 +12094,7 @@
       <c r="Q77" s="135" t="s">
         <v>190</v>
       </c>
-      <c r="R77" s="334">
+      <c r="R77" s="335">
         <v>213</v>
       </c>
       <c r="S77" s="85"/>
@@ -12065,7 +12108,7 @@
       <c r="C78" s="80"/>
       <c r="D78" s="82"/>
       <c r="E78" s="83"/>
-      <c r="F78" s="333"/>
+      <c r="F78" s="334"/>
       <c r="G78" s="134" t="s">
         <v>247</v>
       </c>
@@ -12079,7 +12122,7 @@
       <c r="Q78" s="135" t="s">
         <v>247</v>
       </c>
-      <c r="R78" s="334"/>
+      <c r="R78" s="335"/>
     </row>
     <row r="79" spans="1:80" ht="13.5" customHeight="1" thickBot="1">
       <c r="B79" s="80"/>
@@ -12089,7 +12132,7 @@
         <v/>
       </c>
       <c r="E79" s="100"/>
-      <c r="F79" s="333"/>
+      <c r="F79" s="334"/>
       <c r="G79" s="134" t="s">
         <v>12</v>
       </c>
@@ -12100,7 +12143,7 @@
       <c r="Q79" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="R79" s="334"/>
+      <c r="R79" s="335"/>
       <c r="S79" s="85"/>
       <c r="T79" s="80" t="str">
         <f>IF(T16="","",IF(T16=V12,V14,V12))</f>
@@ -12110,7 +12153,7 @@
     <row r="80" spans="1:80" ht="13.5" customHeight="1" thickBot="1">
       <c r="B80" s="80"/>
       <c r="C80" s="80"/>
-      <c r="D80" s="338">
+      <c r="D80" s="339">
         <v>202</v>
       </c>
       <c r="E80" s="106" t="s">
@@ -12130,12 +12173,12 @@
       <c r="S80" s="107" t="s">
         <v>205</v>
       </c>
-      <c r="T80" s="340">
+      <c r="T80" s="341">
         <v>206</v>
       </c>
     </row>
     <row r="81" spans="4:20" ht="13.5" customHeight="1">
-      <c r="D81" s="333"/>
+      <c r="D81" s="334"/>
       <c r="E81" s="112" t="s">
         <v>208</v>
       </c>
@@ -12156,10 +12199,10 @@
       <c r="S81" s="113" t="s">
         <v>208</v>
       </c>
-      <c r="T81" s="334"/>
+      <c r="T81" s="335"/>
     </row>
     <row r="82" spans="4:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="D82" s="339"/>
+      <c r="D82" s="340"/>
       <c r="E82" s="120" t="s">
         <v>95</v>
       </c>
@@ -12175,7 +12218,7 @@
       <c r="S82" s="126" t="s">
         <v>108</v>
       </c>
-      <c r="T82" s="341"/>
+      <c r="T82" s="342"/>
     </row>
     <row r="83" spans="4:20" ht="13.5" customHeight="1">
       <c r="D83" s="80" t="str">
@@ -12183,7 +12226,7 @@
         <v/>
       </c>
       <c r="E83" s="133"/>
-      <c r="H83" s="333">
+      <c r="H83" s="334">
         <v>221</v>
       </c>
       <c r="I83" s="134" t="s">
@@ -12192,7 +12235,7 @@
       <c r="O83" s="135" t="s">
         <v>215</v>
       </c>
-      <c r="P83" s="334">
+      <c r="P83" s="335">
         <v>222</v>
       </c>
       <c r="S83" s="85"/>
@@ -12206,7 +12249,7 @@
       <c r="E84" s="83"/>
       <c r="F84" s="80"/>
       <c r="G84" s="80"/>
-      <c r="H84" s="333"/>
+      <c r="H84" s="334"/>
       <c r="I84" s="165" t="s">
         <v>250</v>
       </c>
@@ -12219,7 +12262,7 @@
       <c r="O84" s="135" t="s">
         <v>239</v>
       </c>
-      <c r="P84" s="334"/>
+      <c r="P84" s="335"/>
     </row>
     <row r="85" spans="4:20" ht="13.5" customHeight="1" thickBot="1">
       <c r="D85" s="80" t="str">
@@ -12229,14 +12272,14 @@
       <c r="E85" s="100"/>
       <c r="F85" s="80"/>
       <c r="G85" s="80"/>
-      <c r="H85" s="333"/>
+      <c r="H85" s="334"/>
       <c r="I85" s="134" t="s">
         <v>12</v>
       </c>
       <c r="O85" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="P85" s="334"/>
+      <c r="P85" s="335"/>
       <c r="S85" s="85"/>
       <c r="T85" s="86" t="str">
         <f>IF(T28="","",IF(T28=V24,V26,V24))</f>
@@ -12244,7 +12287,7 @@
       </c>
     </row>
     <row r="86" spans="4:20" ht="13.5" customHeight="1">
-      <c r="D86" s="338">
+      <c r="D86" s="339">
         <v>203</v>
       </c>
       <c r="E86" s="106" t="s">
@@ -12259,12 +12302,12 @@
       <c r="S86" s="107" t="s">
         <v>215</v>
       </c>
-      <c r="T86" s="340">
+      <c r="T86" s="341">
         <v>207</v>
       </c>
     </row>
     <row r="87" spans="4:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="D87" s="333"/>
+      <c r="D87" s="334"/>
       <c r="E87" s="112" t="s">
         <v>208</v>
       </c>
@@ -12285,10 +12328,10 @@
       <c r="S87" s="113" t="s">
         <v>234</v>
       </c>
-      <c r="T87" s="334"/>
+      <c r="T87" s="335"/>
     </row>
     <row r="88" spans="4:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="D88" s="339"/>
+      <c r="D88" s="340"/>
       <c r="E88" s="120" t="s">
         <v>100</v>
       </c>
@@ -12296,11 +12339,11 @@
       <c r="G88" s="122"/>
       <c r="H88" s="123"/>
       <c r="I88" s="134"/>
-      <c r="K88" s="342" t="s">
+      <c r="K88" s="343" t="s">
         <v>248</v>
       </c>
-      <c r="L88" s="343"/>
-      <c r="M88" s="343"/>
+      <c r="L88" s="344"/>
+      <c r="M88" s="344"/>
       <c r="O88" s="135"/>
       <c r="P88" s="152"/>
       <c r="Q88" s="124"/>
@@ -12308,7 +12351,7 @@
       <c r="S88" s="126" t="s">
         <v>108</v>
       </c>
-      <c r="T88" s="341"/>
+      <c r="T88" s="342"/>
     </row>
     <row r="89" spans="4:20" ht="13.5" customHeight="1">
       <c r="D89" s="80" t="str">
@@ -12316,7 +12359,7 @@
         <v/>
       </c>
       <c r="E89" s="133"/>
-      <c r="F89" s="333">
+      <c r="F89" s="334">
         <v>212</v>
       </c>
       <c r="G89" s="134" t="s">
@@ -12329,7 +12372,7 @@
       <c r="Q89" s="135" t="s">
         <v>216</v>
       </c>
-      <c r="R89" s="334">
+      <c r="R89" s="335">
         <v>214</v>
       </c>
       <c r="S89" s="85"/>
@@ -12341,7 +12384,7 @@
     <row r="90" spans="4:20" ht="13.5" customHeight="1" thickBot="1">
       <c r="D90" s="178"/>
       <c r="E90" s="83"/>
-      <c r="F90" s="333"/>
+      <c r="F90" s="334"/>
       <c r="G90" s="134" t="s">
         <v>223</v>
       </c>
@@ -12356,7 +12399,7 @@
       <c r="Q90" s="135" t="s">
         <v>223</v>
       </c>
-      <c r="R90" s="334"/>
+      <c r="R90" s="335"/>
     </row>
     <row r="91" spans="4:20" ht="13.5" customHeight="1" thickBot="1">
       <c r="D91" s="80" t="str">
@@ -12364,7 +12407,7 @@
         <v/>
       </c>
       <c r="E91" s="100"/>
-      <c r="F91" s="333"/>
+      <c r="F91" s="334"/>
       <c r="G91" s="134" t="s">
         <v>12</v>
       </c>
@@ -12373,11 +12416,11 @@
       <c r="Q91" s="135" t="s">
         <v>105</v>
       </c>
-      <c r="R91" s="334"/>
+      <c r="R91" s="335"/>
       <c r="S91" s="85"/>
     </row>
     <row r="92" spans="4:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="D92" s="338">
+      <c r="D92" s="339">
         <v>204</v>
       </c>
       <c r="E92" s="106" t="s">
@@ -12388,10 +12431,10 @@
       <c r="I92" s="84"/>
       <c r="Q92" s="153"/>
       <c r="S92" s="188"/>
-      <c r="T92" s="334"/>
+      <c r="T92" s="335"/>
     </row>
     <row r="93" spans="4:20" ht="13.5" customHeight="1">
-      <c r="D93" s="333"/>
+      <c r="D93" s="334"/>
       <c r="E93" s="112" t="s">
         <v>234</v>
       </c>
@@ -12406,10 +12449,10 @@
         <v/>
       </c>
       <c r="S93" s="188"/>
-      <c r="T93" s="334"/>
+      <c r="T93" s="335"/>
     </row>
     <row r="94" spans="4:20" ht="13.5" customHeight="1" thickBot="1">
-      <c r="D94" s="339"/>
+      <c r="D94" s="340"/>
       <c r="E94" s="120" t="s">
         <v>100</v>
       </c>
@@ -12417,7 +12460,7 @@
       <c r="G94" s="80"/>
       <c r="H94" s="84"/>
       <c r="S94" s="188"/>
-      <c r="T94" s="334"/>
+      <c r="T94" s="335"/>
     </row>
     <row r="95" spans="4:20" ht="13.5" customHeight="1">
       <c r="D95" s="80" t="str">
@@ -12462,12 +12505,12 @@
       <c r="G100" s="122"/>
       <c r="H100" s="123"/>
       <c r="I100" s="84"/>
-      <c r="M100" s="333"/>
+      <c r="M100" s="334"/>
       <c r="Q100" s="124"/>
       <c r="R100" s="125"/>
     </row>
     <row r="101" spans="4:50" ht="13.5" customHeight="1">
-      <c r="F101" s="333">
+      <c r="F101" s="334">
         <v>301</v>
       </c>
       <c r="G101" s="191" t="s">
@@ -12475,16 +12518,16 @@
       </c>
       <c r="H101" s="84"/>
       <c r="I101" s="84"/>
-      <c r="M101" s="333"/>
+      <c r="M101" s="334"/>
       <c r="Q101" s="135" t="s">
         <v>216</v>
       </c>
-      <c r="R101" s="334">
+      <c r="R101" s="335">
         <v>303</v>
       </c>
     </row>
     <row r="102" spans="4:50" ht="13.5" customHeight="1" thickBot="1">
-      <c r="F102" s="333"/>
+      <c r="F102" s="334"/>
       <c r="G102" s="191" t="s">
         <v>247</v>
       </c>
@@ -12492,19 +12535,19 @@
         <v>305</v>
       </c>
       <c r="I102" s="84"/>
-      <c r="M102" s="333"/>
+      <c r="M102" s="334"/>
       <c r="P102" s="226" t="s">
         <v>305</v>
       </c>
       <c r="Q102" s="135" t="s">
         <v>224</v>
       </c>
-      <c r="R102" s="334"/>
+      <c r="R102" s="335"/>
       <c r="S102" s="85"/>
       <c r="T102" s="85"/>
     </row>
     <row r="103" spans="4:50" ht="13.5" customHeight="1">
-      <c r="F103" s="333"/>
+      <c r="F103" s="334"/>
       <c r="G103" s="191" t="s">
         <v>12</v>
       </c>
@@ -12515,7 +12558,7 @@
       <c r="Q103" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="R103" s="334"/>
+      <c r="R103" s="335"/>
       <c r="S103" s="85"/>
       <c r="T103" s="85"/>
     </row>
@@ -12568,7 +12611,7 @@
       <c r="T106" s="85"/>
     </row>
     <row r="107" spans="4:50" ht="13.5" customHeight="1">
-      <c r="H107" s="333">
+      <c r="H107" s="334">
         <v>311</v>
       </c>
       <c r="I107" s="134" t="s">
@@ -12580,7 +12623,7 @@
       <c r="O107" s="135" t="s">
         <v>215</v>
       </c>
-      <c r="P107" s="334">
+      <c r="P107" s="335">
         <v>312</v>
       </c>
       <c r="S107" s="85"/>
@@ -12594,7 +12637,7 @@
     <row r="108" spans="4:50" ht="13.5" customHeight="1" thickBot="1">
       <c r="F108" s="80"/>
       <c r="G108" s="80"/>
-      <c r="H108" s="333"/>
+      <c r="H108" s="334"/>
       <c r="I108" s="134" t="s">
         <v>251</v>
       </c>
@@ -12608,7 +12651,7 @@
       <c r="O108" s="135" t="s">
         <v>251</v>
       </c>
-      <c r="P108" s="334"/>
+      <c r="P108" s="335"/>
       <c r="S108" s="85"/>
       <c r="T108" s="85"/>
       <c r="AN108" s="180"/>
@@ -12620,7 +12663,7 @@
     <row r="109" spans="4:50" ht="13.5" customHeight="1">
       <c r="F109" s="80"/>
       <c r="G109" s="80"/>
-      <c r="H109" s="333"/>
+      <c r="H109" s="334"/>
       <c r="I109" s="134" t="s">
         <v>12</v>
       </c>
@@ -12630,7 +12673,7 @@
       <c r="O109" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="P109" s="334"/>
+      <c r="P109" s="335"/>
       <c r="S109" s="85"/>
       <c r="T109" s="85"/>
       <c r="AN109" s="180"/>
@@ -12722,7 +12765,7 @@
       <c r="AX112" s="193"/>
     </row>
     <row r="113" spans="6:50" ht="13.5" customHeight="1">
-      <c r="F113" s="333">
+      <c r="F113" s="334">
         <v>302</v>
       </c>
       <c r="G113" s="134" t="s">
@@ -12735,7 +12778,7 @@
       <c r="Q113" s="135" t="s">
         <v>190</v>
       </c>
-      <c r="R113" s="334">
+      <c r="R113" s="335">
         <v>304</v>
       </c>
       <c r="S113" s="85"/>
@@ -12753,7 +12796,7 @@
       <c r="AX113" s="193"/>
     </row>
     <row r="114" spans="6:50" ht="13.5" customHeight="1" thickBot="1">
-      <c r="F114" s="333"/>
+      <c r="F114" s="334"/>
       <c r="G114" s="134" t="s">
         <v>224</v>
       </c>
@@ -12768,23 +12811,23 @@
       <c r="Q114" s="135" t="s">
         <v>224</v>
       </c>
-      <c r="R114" s="334"/>
+      <c r="R114" s="335"/>
       <c r="S114" s="85"/>
       <c r="T114" s="85"/>
       <c r="AN114" s="180"/>
       <c r="AO114" s="189"/>
-      <c r="AP114" s="335"/>
-      <c r="AQ114" s="337"/>
-      <c r="AR114" s="337"/>
-      <c r="AS114" s="337"/>
-      <c r="AT114" s="337"/>
+      <c r="AP114" s="336"/>
+      <c r="AQ114" s="338"/>
+      <c r="AR114" s="338"/>
+      <c r="AS114" s="338"/>
+      <c r="AT114" s="338"/>
       <c r="AU114" s="192"/>
       <c r="AV114" s="193"/>
       <c r="AW114" s="193"/>
       <c r="AX114" s="193"/>
     </row>
     <row r="115" spans="6:50" ht="13.5" customHeight="1">
-      <c r="F115" s="333"/>
+      <c r="F115" s="334"/>
       <c r="G115" s="134" t="s">
         <v>12</v>
       </c>
@@ -12793,7 +12836,7 @@
       <c r="Q115" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="R115" s="334"/>
+      <c r="R115" s="335"/>
       <c r="S115" s="85"/>
       <c r="T115" s="85"/>
       <c r="AN115" s="180"/>
@@ -12870,11 +12913,11 @@
     <row r="119" spans="6:50" ht="13.5" customHeight="1">
       <c r="AN119" s="180"/>
       <c r="AO119" s="198"/>
-      <c r="AP119" s="335"/>
-      <c r="AQ119" s="336"/>
-      <c r="AR119" s="336"/>
-      <c r="AS119" s="336"/>
-      <c r="AT119" s="336"/>
+      <c r="AP119" s="336"/>
+      <c r="AQ119" s="337"/>
+      <c r="AR119" s="337"/>
+      <c r="AS119" s="337"/>
+      <c r="AT119" s="337"/>
       <c r="AU119" s="192"/>
       <c r="AV119" s="193"/>
       <c r="AW119" s="193"/>
@@ -12924,7 +12967,7 @@
       <c r="G122" s="122"/>
       <c r="H122" s="123"/>
       <c r="I122" s="84"/>
-      <c r="M122" s="333"/>
+      <c r="M122" s="334"/>
       <c r="Q122" s="124"/>
       <c r="R122" s="125"/>
       <c r="AN122" s="180"/>
@@ -12940,7 +12983,7 @@
       <c r="AX122" s="193"/>
     </row>
     <row r="123" spans="6:50" ht="13.5" customHeight="1">
-      <c r="F123" s="333">
+      <c r="F123" s="334">
         <v>401</v>
       </c>
       <c r="G123" s="191" t="s">
@@ -12948,11 +12991,11 @@
       </c>
       <c r="H123" s="84"/>
       <c r="I123" s="84"/>
-      <c r="M123" s="333"/>
+      <c r="M123" s="334"/>
       <c r="Q123" s="135" t="s">
         <v>191</v>
       </c>
-      <c r="R123" s="334">
+      <c r="R123" s="335">
         <v>403</v>
       </c>
       <c r="AN123" s="180"/>
@@ -12968,7 +13011,7 @@
       <c r="AX123" s="193"/>
     </row>
     <row r="124" spans="6:50" ht="13.5" customHeight="1" thickBot="1">
-      <c r="F124" s="333"/>
+      <c r="F124" s="334"/>
       <c r="G124" s="165" t="s">
         <v>250</v>
       </c>
@@ -12976,14 +13019,14 @@
         <v>7</v>
       </c>
       <c r="I124" s="84"/>
-      <c r="M124" s="333"/>
+      <c r="M124" s="334"/>
       <c r="P124" s="226" t="s">
         <v>47</v>
       </c>
       <c r="Q124" s="135" t="s">
         <v>224</v>
       </c>
-      <c r="R124" s="334"/>
+      <c r="R124" s="335"/>
       <c r="AN124" s="180"/>
       <c r="AO124" s="197"/>
       <c r="AP124" s="196"/>
@@ -12997,7 +13040,7 @@
       <c r="AX124" s="193"/>
     </row>
     <row r="125" spans="6:50" ht="13.5" customHeight="1">
-      <c r="F125" s="333"/>
+      <c r="F125" s="334"/>
       <c r="G125" s="191" t="s">
         <v>12</v>
       </c>
@@ -13008,7 +13051,7 @@
       <c r="Q125" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="R125" s="334"/>
+      <c r="R125" s="335"/>
       <c r="AN125" s="180"/>
       <c r="AO125" s="198"/>
       <c r="AP125" s="196"/>
@@ -13035,11 +13078,11 @@
       <c r="R126" s="154"/>
       <c r="AN126" s="180"/>
       <c r="AO126" s="198"/>
-      <c r="AP126" s="335"/>
-      <c r="AQ126" s="336"/>
-      <c r="AR126" s="336"/>
-      <c r="AS126" s="336"/>
-      <c r="AT126" s="336"/>
+      <c r="AP126" s="336"/>
+      <c r="AQ126" s="337"/>
+      <c r="AR126" s="337"/>
+      <c r="AS126" s="337"/>
+      <c r="AT126" s="337"/>
       <c r="AU126" s="192"/>
       <c r="AV126" s="193"/>
       <c r="AW126" s="193"/>
@@ -13097,7 +13140,7 @@
       <c r="AX128" s="193"/>
     </row>
     <row r="129" spans="6:50" ht="13.5" customHeight="1">
-      <c r="H129" s="333">
+      <c r="H129" s="334">
         <v>411</v>
       </c>
       <c r="I129" s="134" t="s">
@@ -13109,7 +13152,7 @@
       <c r="O129" s="135" t="s">
         <v>190</v>
       </c>
-      <c r="P129" s="334">
+      <c r="P129" s="335">
         <v>412</v>
       </c>
       <c r="AN129" s="180"/>
@@ -13127,7 +13170,7 @@
     <row r="130" spans="6:50" ht="13.5" customHeight="1" thickBot="1">
       <c r="F130" s="80"/>
       <c r="G130" s="80"/>
-      <c r="H130" s="333"/>
+      <c r="H130" s="334"/>
       <c r="I130" s="134" t="s">
         <v>251</v>
       </c>
@@ -13139,14 +13182,14 @@
       <c r="O130" s="135" t="s">
         <v>251</v>
       </c>
-      <c r="P130" s="334"/>
+      <c r="P130" s="335"/>
       <c r="AN130" s="180"/>
       <c r="AO130" s="198"/>
-      <c r="AP130" s="335"/>
-      <c r="AQ130" s="336"/>
-      <c r="AR130" s="336"/>
-      <c r="AS130" s="336"/>
-      <c r="AT130" s="336"/>
+      <c r="AP130" s="336"/>
+      <c r="AQ130" s="337"/>
+      <c r="AR130" s="337"/>
+      <c r="AS130" s="337"/>
+      <c r="AT130" s="337"/>
       <c r="AU130" s="192"/>
       <c r="AV130" s="193"/>
       <c r="AW130" s="193"/>
@@ -13155,7 +13198,7 @@
     <row r="131" spans="6:50" ht="13.5" customHeight="1">
       <c r="F131" s="80"/>
       <c r="G131" s="80"/>
-      <c r="H131" s="333"/>
+      <c r="H131" s="334"/>
       <c r="I131" s="134" t="s">
         <v>12</v>
       </c>
@@ -13165,7 +13208,7 @@
       <c r="O131" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="P131" s="334"/>
+      <c r="P131" s="335"/>
       <c r="AN131" s="180"/>
       <c r="AO131" s="197"/>
       <c r="AP131" s="196"/>
@@ -13242,18 +13285,18 @@
       <c r="R134" s="125"/>
       <c r="AN134" s="180"/>
       <c r="AO134" s="189"/>
-      <c r="AP134" s="331"/>
-      <c r="AQ134" s="332"/>
-      <c r="AR134" s="331"/>
-      <c r="AS134" s="332"/>
-      <c r="AT134" s="331"/>
-      <c r="AU134" s="332"/>
-      <c r="AV134" s="331"/>
-      <c r="AW134" s="332"/>
+      <c r="AP134" s="332"/>
+      <c r="AQ134" s="333"/>
+      <c r="AR134" s="332"/>
+      <c r="AS134" s="333"/>
+      <c r="AT134" s="332"/>
+      <c r="AU134" s="333"/>
+      <c r="AV134" s="332"/>
+      <c r="AW134" s="333"/>
       <c r="AX134" s="193"/>
     </row>
     <row r="135" spans="6:50" ht="13.5" customHeight="1">
-      <c r="F135" s="333">
+      <c r="F135" s="334">
         <v>402</v>
       </c>
       <c r="G135" s="134" t="s">
@@ -13266,7 +13309,7 @@
       <c r="Q135" s="135" t="s">
         <v>191</v>
       </c>
-      <c r="R135" s="334">
+      <c r="R135" s="335">
         <v>404</v>
       </c>
       <c r="AN135" s="180"/>
@@ -13282,7 +13325,7 @@
       <c r="AX135" s="193"/>
     </row>
     <row r="136" spans="6:50" ht="13.5" customHeight="1" thickBot="1">
-      <c r="F136" s="333"/>
+      <c r="F136" s="334"/>
       <c r="G136" s="134" t="s">
         <v>224</v>
       </c>
@@ -13297,7 +13340,7 @@
       <c r="Q136" s="135" t="s">
         <v>250</v>
       </c>
-      <c r="R136" s="334"/>
+      <c r="R136" s="335"/>
       <c r="AN136" s="180"/>
       <c r="AO136" s="189"/>
       <c r="AP136" s="142"/>
@@ -13311,7 +13354,7 @@
       <c r="AX136" s="193"/>
     </row>
     <row r="137" spans="6:50" ht="13.5" customHeight="1">
-      <c r="F137" s="333"/>
+      <c r="F137" s="334"/>
       <c r="G137" s="134" t="s">
         <v>12</v>
       </c>
@@ -13320,7 +13363,7 @@
       <c r="Q137" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="R137" s="334"/>
+      <c r="R137" s="335"/>
       <c r="AN137" s="180"/>
       <c r="AO137" s="189"/>
       <c r="AP137" s="142"/>
@@ -13652,10 +13695,10 @@
       <c r="AQ154" s="193"/>
       <c r="AR154" s="163"/>
       <c r="AS154" s="193"/>
-      <c r="AT154" s="331"/>
-      <c r="AU154" s="332"/>
-      <c r="AV154" s="331"/>
-      <c r="AW154" s="332"/>
+      <c r="AT154" s="332"/>
+      <c r="AU154" s="333"/>
+      <c r="AV154" s="332"/>
+      <c r="AW154" s="333"/>
       <c r="AX154" s="193"/>
     </row>
     <row r="155" spans="6:50" ht="13.5" customHeight="1">
@@ -14121,10 +14164,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="22.9" customHeight="1">
-      <c r="A4" s="364" t="s">
+      <c r="A4" s="365" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="365"/>
+      <c r="B4" s="366"/>
       <c r="C4" s="232" t="s">
         <v>274</v>
       </c>
@@ -14163,10 +14206,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="22.9" customHeight="1">
-      <c r="C8" s="366" t="s">
+      <c r="C8" s="367" t="s">
         <v>283</v>
       </c>
-      <c r="D8" s="366"/>
+      <c r="D8" s="367"/>
     </row>
     <row r="9" spans="1:7" ht="22.9" customHeight="1">
       <c r="B9" s="232" t="s">
@@ -14178,11 +14221,11 @@
       <c r="D9" s="232" t="s">
         <v>277</v>
       </c>
-      <c r="E9" s="364" t="s">
+      <c r="E9" s="365" t="s">
         <v>278</v>
       </c>
-      <c r="F9" s="365"/>
-      <c r="G9" s="365"/>
+      <c r="F9" s="366"/>
+      <c r="G9" s="366"/>
     </row>
     <row r="10" spans="1:7" ht="22.9" customHeight="1" thickBot="1">
       <c r="A10" s="232" t="s">

</xml_diff>